<commit_message>
Changes in the Script
</commit_message>
<xml_diff>
--- a/Iseek/src/resources/TestData/Data.xlsx
+++ b/Iseek/src/resources/TestData/Data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Password</t>
   </si>
@@ -44,9 +44,6 @@
     <t>OfferName</t>
   </si>
   <si>
-    <t>2/22/2019</t>
-  </si>
-  <si>
     <t>Iseek</t>
   </si>
   <si>
@@ -63,6 +60,27 @@
   </si>
   <si>
     <t>Default Testing</t>
+  </si>
+  <si>
+    <t>Iseek2</t>
+  </si>
+  <si>
+    <t>Testing3</t>
+  </si>
+  <si>
+    <t>Start_Date</t>
+  </si>
+  <si>
+    <t>2/12/2019</t>
+  </si>
+  <si>
+    <t>12/31/2019</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>2500</t>
   </si>
 </sst>
 </file>
@@ -473,22 +491,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -496,37 +515,75 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="2" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>